<commit_message>
Seniority functionality for SMs and todo list
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/WS02-schedule-wishes-Jan-6th-12th_Sven.xlsx
+++ b/Graafikuseedija/src/WS02-schedule-wishes-Jan-6th-12th_Sven.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1f3b2b2e0b977bc/Documents/graafikuseedija/Graafikuseedija/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC78BA12-20B4-4EC0-8D3D-AA985714D4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{DC78BA12-20B4-4EC0-8D3D-AA985714D4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2A29CE5-69C4-4AFF-A73F-8AD47C56E8F8}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="1515" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="450" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Anne-Mai Pall</t>
   </si>
   <si>
-    <t>Martin Merisalu</t>
-  </si>
-  <si>
     <t>Rasmus Rahnu</t>
   </si>
   <si>
@@ -174,16 +171,34 @@
     <t>Helena Jallai</t>
   </si>
   <si>
-    <t>Siim Pari</t>
-  </si>
-  <si>
-    <t>Marko Lepamets</t>
-  </si>
-  <si>
     <t>Siia panin 2 nime manuaalselt juurde</t>
   </si>
   <si>
     <t>Shift Manageri vahetusi peaks lihtsalt ignoreerima</t>
+  </si>
+  <si>
+    <t>SMMartin Merisalu</t>
+  </si>
+  <si>
+    <t>SMMarko Lepamets</t>
+  </si>
+  <si>
+    <t>SMSiim Pari</t>
+  </si>
+  <si>
+    <t>Peeter Talutagune</t>
+  </si>
+  <si>
+    <t>Meeter Taluesine</t>
+  </si>
+  <si>
+    <t>Kalle Plonkvist</t>
+  </si>
+  <si>
+    <t>Karlsson Katuselt</t>
+  </si>
+  <si>
+    <t>Tiiu Maalt</t>
   </si>
 </sst>
 </file>
@@ -295,8 +310,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M26" totalsRowShown="0">
-  <autoFilter ref="A1:M26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0">
+  <autoFilter ref="A1:M31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="11"/>
@@ -613,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,12 +720,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
@@ -1026,7 +1041,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>18</v>
@@ -1053,7 +1068,7 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
@@ -1086,7 +1101,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1119,7 +1134,7 @@
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
@@ -1152,7 +1167,7 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1183,7 +1198,7 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
@@ -1218,7 +1233,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>13</v>
@@ -1255,7 +1270,7 @@
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1284,7 +1299,7 @@
         <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1308,12 +1323,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1346,7 +1361,7 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
@@ -1373,7 +1388,7 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
@@ -1413,11 +1428,11 @@
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1427,6 +1442,91 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
All names now have the first letter of their last name added. Parser, reduced the switch cases from 21 to 3, Changed worker class drastically, now instead of having a value for each day, the object has all of them in a list. This allowed me to reimagine the Parses class into something that is much more efficient and usable. Parser, added a new method for checking the availability of the worker writeToXML, added a new method to for inputing cells into the xslx file. readFromXML, made changes so that it can work with the new worker class.
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/WS02-schedule-wishes-Jan-6th-12th_Sven.xlsx
+++ b/Graafikuseedija/src/WS02-schedule-wishes-Jan-6th-12th_Sven.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1f3b2b2e0b977bc/Documents/graafikuseedija/Graafikuseedija/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{DC78BA12-20B4-4EC0-8D3D-AA985714D4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2A29CE5-69C4-4AFF-A73F-8AD47C56E8F8}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{DC78BA12-20B4-4EC0-8D3D-AA985714D4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BED9DA5B-475E-4445-9DFE-C2DAC93CCF59}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="450" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="300" windowWidth="23205" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -114,15 +114,9 @@
     <t>Siim Lillemets</t>
   </si>
   <si>
-    <t>Joonas Karl Kuusik</t>
-  </si>
-  <si>
     <t>Madis Klesment</t>
   </si>
   <si>
-    <t>Daniell Sepp</t>
-  </si>
-  <si>
     <t>Helena Mandel</t>
   </si>
   <si>
@@ -171,34 +165,37 @@
     <t>Helena Jallai</t>
   </si>
   <si>
-    <t>Siia panin 2 nime manuaalselt juurde</t>
-  </si>
-  <si>
     <t>Shift Manageri vahetusi peaks lihtsalt ignoreerima</t>
   </si>
   <si>
-    <t>SMMartin Merisalu</t>
-  </si>
-  <si>
     <t>SMMarko Lepamets</t>
   </si>
   <si>
     <t>SMSiim Pari</t>
   </si>
   <si>
-    <t>Peeter Talutagune</t>
-  </si>
-  <si>
-    <t>Meeter Taluesine</t>
-  </si>
-  <si>
-    <t>Kalle Plonkvist</t>
-  </si>
-  <si>
-    <t>Karlsson Katuselt</t>
-  </si>
-  <si>
-    <t>Tiiu Maalt</t>
+    <t>Buse Erdem</t>
+  </si>
+  <si>
+    <t>Daniell Lepp</t>
+  </si>
+  <si>
+    <t>Joonas Kari Kuusik</t>
+  </si>
+  <si>
+    <t>SMJuulia Kaas</t>
+  </si>
+  <si>
+    <t>Kristjan Kaljurand</t>
+  </si>
+  <si>
+    <t>Martin Merisalu</t>
+  </si>
+  <si>
+    <t>Shawn Michael Rains</t>
+  </si>
+  <si>
+    <t>Siia panin nimesid manuaalselt juurde</t>
   </si>
 </sst>
 </file>
@@ -310,22 +307,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M31" totalsRowShown="0">
-  <autoFilter ref="A1:M31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{67E872F0-87EB-494D-8CDD-8726449488F4}" name="Table13" displayName="Table13" ref="A1:M31" totalsRowShown="0">
+  <autoFilter ref="A1:M31" xr:uid="{2446CA85-39FE-4E3B-8DD2-108608D23874}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Monday" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tuesday" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wednesday" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Thursday" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Friday" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Saturday" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Sunday" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2B6483BE-7FCB-4FAB-98BE-F3258D13DB3C}" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{9942BDFA-6ECD-4738-AE66-BBDD45CF9C0E}" name="Start time" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{32E105DD-2FF5-4FFB-AE89-76936C21530B}" name="Completion time" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B53F91AA-B2D6-46FD-992C-4EC97B8763FD}" name="Email" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DB0939C0-F8A3-482E-9D29-BE28D3AA3122}" name="Name" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{597B7D54-B29A-4C92-BB96-1495DB7EE28B}" name="Monday" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{39C13870-B3EC-4E39-806E-7A2042A5C616}" name="Tuesday" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{F983EC72-5710-4135-9305-3BAAEE02FFE2}" name="Wednesday" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{B41F01A0-3ED0-4951-B73E-360DF186430E}" name="Thursday" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{A436D1FE-BC3D-461A-BB2F-49E01E068FA8}" name="Friday" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{0283F323-05FF-4D04-A039-C8FA26B380A9}" name="Saturday" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{BEC90A9D-4A19-42E0-8D7E-6B4B99E28072}" name="Sunday" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{1FB4AD32-079B-4EA4-AC0D-C7A984A43811}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -627,11 +624,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B99A2D-2CAF-4BBB-8769-CB25A6BB6D84}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +691,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
@@ -720,12 +717,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
@@ -756,7 +753,7 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
@@ -785,7 +782,7 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -816,7 +813,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -847,7 +844,7 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
@@ -884,7 +881,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>21</v>
@@ -921,7 +918,7 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -950,7 +947,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -979,7 +976,7 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1010,7 +1007,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1041,7 +1038,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>18</v>
@@ -1068,7 +1065,7 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>16</v>
@@ -1101,7 +1098,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1134,7 +1131,7 @@
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
@@ -1167,7 +1164,7 @@
         <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1198,7 +1195,7 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
@@ -1233,7 +1230,7 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>13</v>
@@ -1270,7 +1267,7 @@
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1299,7 +1296,7 @@
         <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1323,12 +1320,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1361,7 +1358,7 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
@@ -1388,7 +1385,7 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
@@ -1428,11 +1425,11 @@
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1449,7 +1446,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1466,7 +1463,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1483,7 +1480,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1500,7 +1497,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1516,9 +1513,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1530,12 +1525,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{9698D592-6960-42D0-96E9-4EFFCA1C2CD5}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6E6CB96A-169F-405D-B0FB-11D7ED339F62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>